<commit_message>
Add rotate and zoom preprocessing
</commit_message>
<xml_diff>
--- a/reports/image_preprocessing_results.xlsx
+++ b/reports/image_preprocessing_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Masters\ISSS610 Applied Machine Learning\Project\chexpert-aml\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{151DE4EF-1021-4487-A4B5-499AAB04B5DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD860AEB-5A6D-45C7-BE02-EB4980BD92B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="66">
   <si>
     <t>args</t>
   </si>
@@ -153,6 +153,60 @@
   </si>
   <si>
     <t>[['crop', {'size': [320, 320]}], ['eqhist', {}], ['gaussian_blur', {}], ['normalize', {}], ['flatten', {}]]</t>
+  </si>
+  <si>
+    <t>Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_median_blur_normalize_rotate.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])</t>
+  </si>
+  <si>
+    <t>[['crop', {'size': [320, 320]}], ['median_blur', {}], ['normalize', {}], ['rotate', {}], ['flatten', {}]]</t>
+  </si>
+  <si>
+    <t>Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_rotate.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])</t>
+  </si>
+  <si>
+    <t>[['crop', {'size': [320, 320]}], ['eqhist', {}], ['rotate', {}], ['flatten', {}]]</t>
+  </si>
+  <si>
+    <t>Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_median_blur_rotate.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])</t>
+  </si>
+  <si>
+    <t>[['crop', {'size': [320, 320]}], ['eqhist', {}], ['median_blur', {}], ['rotate', {}], ['flatten', {}]]</t>
+  </si>
+  <si>
+    <t>Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_median_blur_normalize_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])</t>
+  </si>
+  <si>
+    <t>[['crop', {'size': [320, 320]}], ['median_blur', {}], ['normalize', {}], ['zoom', {}], ['flatten', {}]]</t>
+  </si>
+  <si>
+    <t>Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_median_blur_normalize_rotate_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])</t>
+  </si>
+  <si>
+    <t>[['crop', {'size': [320, 320]}], ['median_blur', {}], ['normalize', {}], ['rotate', {}], ['zoom', {}], ['flatten', {}]]</t>
+  </si>
+  <si>
+    <t>Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])</t>
+  </si>
+  <si>
+    <t>[['crop', {'size': [320, 320]}], ['eqhist', {}], ['zoom', {}], ['flatten', {}]]</t>
+  </si>
+  <si>
+    <t>Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_rotate_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])</t>
+  </si>
+  <si>
+    <t>[['crop', {'size': [320, 320]}], ['eqhist', {}], ['rotate', {}], ['zoom', {}], ['flatten', {}]]</t>
+  </si>
+  <si>
+    <t>Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_median_blur_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])</t>
+  </si>
+  <si>
+    <t>[['crop', {'size': [320, 320]}], ['eqhist', {}], ['median_blur', {}], ['zoom', {}], ['flatten', {}]]</t>
+  </si>
+  <si>
+    <t>Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_median_blur_rotate_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])</t>
+  </si>
+  <si>
+    <t>[['crop', {'size': [320, 320]}], ['eqhist', {}], ['median_blur', {}], ['rotate', {}], ['zoom', {}], ['flatten', {}]]</t>
   </si>
   <si>
     <t>Row Labels</t>
@@ -658,10 +712,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -707,7 +759,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="10">
     <dxf>
       <font>
         <b val="0"/>
@@ -777,6 +829,102 @@
         <patternFill patternType="solid">
           <fgColor indexed="65"/>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF9C5700"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="65"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF9C5700"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="65"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF9C5700"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="65"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF9C5700"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="65"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -866,16 +1014,16 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Administrator" refreshedDate="44399.479234259263" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="80">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Administrator" refreshedDate="44400.043607754633" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="125">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:F81" sheet="image_preprocessing_results"/>
+    <worksheetSource ref="A1:F126" sheet="image_preprocessing_results"/>
   </cacheSource>
   <cacheFields count="6">
     <cacheField name="args" numFmtId="0">
       <sharedItems longText="1"/>
     </cacheField>
     <cacheField name="preprocessing" numFmtId="0">
-      <sharedItems count="16">
+      <sharedItems count="25">
         <s v="[['crop', {'size': [320, 320]}], ['flatten', {}]]"/>
         <s v="[['resize', {'size': [320, 320]}], ['flatten', {}]]"/>
         <s v="[['crop', {'size': [320, 320]}], ['median_blur', {}], ['flatten', {}]]"/>
@@ -892,19 +1040,28 @@
         <s v="[['crop', {'size': [320, 320]}], ['adaptive_eqhist', {}], ['normalize', {}], ['flatten', {}]]"/>
         <s v="[['crop', {'size': [320, 320]}], ['eqhist', {}], ['median_blur', {}], ['normalize', {}], ['flatten', {}]]"/>
         <s v="[['crop', {'size': [320, 320]}], ['eqhist', {}], ['gaussian_blur', {}], ['normalize', {}], ['flatten', {}]]"/>
+        <s v="[['crop', {'size': [320, 320]}], ['median_blur', {}], ['normalize', {}], ['rotate', {}], ['flatten', {}]]"/>
+        <s v="[['crop', {'size': [320, 320]}], ['eqhist', {}], ['rotate', {}], ['flatten', {}]]"/>
+        <s v="[['crop', {'size': [320, 320]}], ['eqhist', {}], ['median_blur', {}], ['rotate', {}], ['flatten', {}]]"/>
+        <s v="[['crop', {'size': [320, 320]}], ['median_blur', {}], ['normalize', {}], ['zoom', {}], ['flatten', {}]]"/>
+        <s v="[['crop', {'size': [320, 320]}], ['median_blur', {}], ['normalize', {}], ['rotate', {}], ['zoom', {}], ['flatten', {}]]"/>
+        <s v="[['crop', {'size': [320, 320]}], ['eqhist', {}], ['zoom', {}], ['flatten', {}]]"/>
+        <s v="[['crop', {'size': [320, 320]}], ['eqhist', {}], ['rotate', {}], ['zoom', {}], ['flatten', {}]]"/>
+        <s v="[['crop', {'size': [320, 320]}], ['eqhist', {}], ['median_blur', {}], ['zoom', {}], ['flatten', {}]]"/>
+        <s v="[['crop', {'size': [320, 320]}], ['eqhist', {}], ['median_blur', {}], ['rotate', {}], ['zoom', {}], ['flatten', {}]]"/>
       </sharedItems>
     </cacheField>
     <cacheField name="label" numFmtId="0">
       <sharedItems/>
     </cacheField>
     <cacheField name="roc_auc_score" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.32646103896103901" maxValue="0.73175053153791603"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.32646103900000001" maxValue="0.73281360699999998"/>
     </cacheField>
     <cacheField name="accuracy" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.51282051299999998" maxValue="0.854700854700854"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.51282051299999998" maxValue="0.85470085500000004"/>
     </cacheField>
     <cacheField name="f1_score" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="0.5625"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="0.57342657299999999"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -916,7 +1073,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="80">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="125">
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="0"/>
@@ -1241,332 +1398,692 @@
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="8"/>
     <s v="Atelectasis"/>
-    <n v="0.63457792207792196"/>
-    <n v="0.59401709401709402"/>
-    <n v="0.53658536585365801"/>
+    <n v="0.63457792199999996"/>
+    <n v="0.59401709400000002"/>
+    <n v="0.53658536599999995"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="8"/>
     <s v="Cardiomegaly"/>
-    <n v="0.71305811481218995"/>
-    <n v="0.683760683760683"/>
+    <n v="0.71305811500000005"/>
+    <n v="0.68376068400000001"/>
     <n v="0.53749999999999998"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="8"/>
     <s v="Consolidation"/>
-    <n v="0.64601236243027205"/>
-    <n v="0.69230769230769196"/>
-    <n v="0.33333333333333298"/>
+    <n v="0.64601236200000001"/>
+    <n v="0.69230769199999997"/>
+    <n v="0.33333333300000001"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="8"/>
     <s v="Edema"/>
-    <n v="0.65802469135802399"/>
-    <n v="0.55982905982905895"/>
-    <n v="0.390532544378698"/>
+    <n v="0.65802469100000005"/>
+    <n v="0.55982905999999999"/>
+    <n v="0.39053254399999998"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="8"/>
     <s v="Pleural Effusion"/>
-    <n v="0.65747609259093698"/>
-    <n v="0.63675213675213604"/>
-    <n v="0.47204968944099301"/>
+    <n v="0.65747609299999998"/>
+    <n v="0.636752137"/>
+    <n v="0.47204968899999999"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\resize_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="9"/>
     <s v="Atelectasis"/>
-    <n v="0.34537337662337603"/>
-    <n v="0.61111111111111105"/>
+    <n v="0.34537337699999998"/>
+    <n v="0.61111111100000004"/>
     <n v="0"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\resize_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="9"/>
     <s v="Cardiomegaly"/>
-    <n v="0.42762225372076501"/>
-    <n v="0.67948717948717896"/>
-    <n v="2.5974025974025899E-2"/>
+    <n v="0.42762225399999998"/>
+    <n v="0.679487179"/>
+    <n v="2.5974026000000001E-2"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\resize_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="9"/>
     <s v="Consolidation"/>
-    <n v="0.41579978893411701"/>
-    <n v="0.854700854700854"/>
+    <n v="0.41579978899999998"/>
+    <n v="0.85470085500000004"/>
     <n v="0"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\resize_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="9"/>
     <s v="Edema"/>
-    <n v="0.452674897119341"/>
-    <n v="0.76068376068375998"/>
-    <n v="3.4482758620689599E-2"/>
+    <n v="0.45267489700000002"/>
+    <n v="0.76068376100000001"/>
+    <n v="3.4482759000000002E-2"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\resize_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="9"/>
     <s v="Pleural Effusion"/>
-    <n v="0.49888283135222"/>
-    <n v="0.658119658119658"/>
-    <n v="6.9767441860465101E-2"/>
+    <n v="0.49888283100000003"/>
+    <n v="0.65811965800000005"/>
+    <n v="6.9767441999999999E-2"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_median_blur_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="10"/>
     <s v="Atelectasis"/>
-    <n v="0.63835227272727202"/>
-    <n v="0.60256410256410198"/>
-    <n v="0.53266331658291399"/>
+    <n v="0.63835227299999997"/>
+    <n v="0.60256410299999996"/>
+    <n v="0.53266331700000003"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_median_blur_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="10"/>
     <s v="Cardiomegaly"/>
-    <n v="0.73175053153791603"/>
-    <n v="0.70085470085470003"/>
+    <n v="0.73175053199999995"/>
+    <n v="0.70085470100000002"/>
     <n v="0.5625"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_median_blur_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="10"/>
     <s v="Consolidation"/>
-    <n v="0.71702095582692604"/>
-    <n v="0.67948717948717896"/>
-    <n v="0.369747899159663"/>
+    <n v="0.71702095600000004"/>
+    <n v="0.679487179"/>
+    <n v="0.36974789899999999"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_median_blur_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="10"/>
     <s v="Edema"/>
-    <n v="0.68165784832451504"/>
-    <n v="0.59829059829059805"/>
+    <n v="0.68165784799999996"/>
+    <n v="0.59829059799999995"/>
     <n v="0.41249999999999998"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_median_blur_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="10"/>
     <s v="Pleural Effusion"/>
-    <n v="0.67164179104477595"/>
-    <n v="0.63675213675213604"/>
-    <n v="0.47852760736196298"/>
+    <n v="0.67164179099999999"/>
+    <n v="0.636752137"/>
+    <n v="0.47852760700000002"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_gaussian_blur_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="11"/>
     <s v="Atelectasis"/>
-    <n v="0.34082792207792201"/>
-    <n v="0.61538461538461497"/>
-    <n v="2.1739130434782601E-2"/>
+    <n v="0.34082792200000001"/>
+    <n v="0.61538461499999997"/>
+    <n v="2.1739129999999999E-2"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_gaussian_blur_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="11"/>
     <s v="Cardiomegaly"/>
-    <n v="0.43320340184266398"/>
-    <n v="0.67521367521367504"/>
+    <n v="0.43320340200000002"/>
+    <n v="0.67521367499999996"/>
     <n v="0"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_gaussian_blur_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="11"/>
     <s v="Consolidation"/>
-    <n v="0.42740841248303901"/>
-    <n v="0.854700854700854"/>
+    <n v="0.42740841200000002"/>
+    <n v="0.85470085500000004"/>
     <n v="0"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_gaussian_blur_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="11"/>
     <s v="Edema"/>
-    <n v="0.463609641387419"/>
-    <n v="0.77777777777777701"/>
-    <n v="0.133333333333333"/>
+    <n v="0.46360964100000002"/>
+    <n v="0.77777777800000003"/>
+    <n v="0.133333333"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_gaussian_blur_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="11"/>
     <s v="Pleural Effusion"/>
-    <n v="0.48404683170971402"/>
-    <n v="0.65384615384615297"/>
-    <n v="6.8965517241379296E-2"/>
+    <n v="0.48404683199999998"/>
+    <n v="0.65384615400000001"/>
+    <n v="6.8965517000000004E-2"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="12"/>
     <s v="Atelectasis"/>
-    <n v="0.32694805194805199"/>
-    <n v="0.60683760683760601"/>
+    <n v="0.32694805199999999"/>
+    <n v="0.606837607"/>
     <n v="0"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="12"/>
     <s v="Cardiomegaly"/>
-    <n v="0.41087880935506699"/>
-    <n v="0.66666666666666596"/>
+    <n v="0.41087880900000001"/>
+    <n v="0.66666666699999999"/>
     <n v="0"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="12"/>
     <s v="Consolidation"/>
-    <n v="0.40524649479873298"/>
-    <n v="0.841880341880341"/>
+    <n v="0.40524649499999998"/>
+    <n v="0.84188034199999995"/>
     <n v="0"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="12"/>
     <s v="Edema"/>
-    <n v="0.44832451499118098"/>
-    <n v="0.75641025641025605"/>
-    <n v="6.5573770491803199E-2"/>
+    <n v="0.44832451499999998"/>
+    <n v="0.756410256"/>
+    <n v="6.5573770000000003E-2"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="12"/>
     <s v="Pleural Effusion"/>
-    <n v="0.55813745643042201"/>
-    <n v="0.66239316239316204"/>
-    <n v="0.168421052631578"/>
+    <n v="0.55813745599999998"/>
+    <n v="0.66239316199999998"/>
+    <n v="0.16842105299999999"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_adaptive_eqhist_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="13"/>
     <s v="Atelectasis"/>
-    <n v="0.36899350649350598"/>
-    <n v="0.60256410256410198"/>
-    <n v="4.1237113402061799E-2"/>
+    <n v="0.36899350600000003"/>
+    <n v="0.60256410299999996"/>
+    <n v="4.1237112999999999E-2"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_adaptive_eqhist_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="13"/>
     <s v="Cardiomegaly"/>
-    <n v="0.43594968107725002"/>
-    <n v="0.66666666666666596"/>
-    <n v="4.8780487804878002E-2"/>
+    <n v="0.43594968099999998"/>
+    <n v="0.66666666699999999"/>
+    <n v="4.8780487999999997E-2"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_adaptive_eqhist_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="13"/>
     <s v="Consolidation"/>
-    <n v="0.42921754862053302"/>
-    <n v="0.841880341880341"/>
+    <n v="0.42921754899999998"/>
+    <n v="0.84188034199999995"/>
     <n v="0"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_adaptive_eqhist_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="13"/>
     <s v="Edema"/>
-    <n v="0.44291593180481997"/>
-    <n v="0.75641025641025605"/>
-    <n v="9.5238095238095205E-2"/>
+    <n v="0.44291593200000001"/>
+    <n v="0.756410256"/>
+    <n v="9.5238094999999995E-2"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_adaptive_eqhist_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="13"/>
     <s v="Pleural Effusion"/>
-    <n v="0.39404772544463301"/>
-    <n v="0.66239316239316204"/>
-    <n v="7.0588235294117604E-2"/>
+    <n v="0.39404772500000002"/>
+    <n v="0.66239316199999998"/>
+    <n v="7.0588234999999999E-2"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_median_blur_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="14"/>
     <s v="Atelectasis"/>
-    <n v="0.32930194805194801"/>
-    <n v="0.60683760683760601"/>
+    <n v="0.32930194800000001"/>
+    <n v="0.606837607"/>
     <n v="0"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_median_blur_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="14"/>
     <s v="Cardiomegaly"/>
-    <n v="0.40786676116229598"/>
-    <n v="0.67948717948717896"/>
+    <n v="0.40786676100000002"/>
+    <n v="0.679487179"/>
     <n v="0"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_median_blur_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="14"/>
     <s v="Consolidation"/>
-    <n v="0.40419116538519501"/>
-    <n v="0.841880341880341"/>
+    <n v="0.40419116500000002"/>
+    <n v="0.84188034199999995"/>
     <n v="0"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_median_blur_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="14"/>
     <s v="Edema"/>
-    <n v="0.444914756025867"/>
-    <n v="0.76068376068375998"/>
-    <n v="6.6666666666666596E-2"/>
+    <n v="0.44491475600000002"/>
+    <n v="0.76068376100000001"/>
+    <n v="6.6666666999999999E-2"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_median_blur_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="14"/>
     <s v="Pleural Effusion"/>
-    <n v="0.47224953078916698"/>
-    <n v="0.66666666666666596"/>
-    <n v="9.3023255813953404E-2"/>
+    <n v="0.472249531"/>
+    <n v="0.66666666699999999"/>
+    <n v="9.3023255999999999E-2"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_gaussian_blur_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="15"/>
     <s v="Atelectasis"/>
-    <n v="0.32646103896103901"/>
-    <n v="0.61111111111111105"/>
+    <n v="0.32646103900000001"/>
+    <n v="0.61111111100000004"/>
     <n v="0"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_gaussian_blur_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="15"/>
     <s v="Cardiomegaly"/>
-    <n v="0.41123316796598097"/>
-    <n v="0.67094017094017"/>
+    <n v="0.41123316799999998"/>
+    <n v="0.67094017100000003"/>
     <n v="0"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_gaussian_blur_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="15"/>
     <s v="Consolidation"/>
-    <n v="0.40434192672998598"/>
-    <n v="0.83760683760683696"/>
+    <n v="0.40434192699999999"/>
+    <n v="0.83760683800000002"/>
     <n v="0"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_gaussian_blur_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="15"/>
     <s v="Edema"/>
-    <n v="0.44456202233980002"/>
-    <n v="0.75641025641025605"/>
-    <n v="6.5573770491803199E-2"/>
+    <n v="0.444562022"/>
+    <n v="0.756410256"/>
+    <n v="6.5573770000000003E-2"/>
   </r>
   <r>
     <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_gaussian_blur_normalize.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
     <x v="15"/>
     <s v="Pleural Effusion"/>
-    <n v="0.50388774689427096"/>
-    <n v="0.66239316239316204"/>
-    <n v="9.1954022988505704E-2"/>
+    <n v="0.50388774700000005"/>
+    <n v="0.66239316199999998"/>
+    <n v="9.1954022999999996E-2"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_median_blur_normalize_rotate.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="16"/>
+    <s v="Atelectasis"/>
+    <n v="0.59066558400000002"/>
+    <n v="0.54273504299999997"/>
+    <n v="0.45685279200000001"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_median_blur_normalize_rotate.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="16"/>
+    <s v="Cardiomegaly"/>
+    <n v="0.69472005699999995"/>
+    <n v="0.66239316199999998"/>
+    <n v="0.52121212100000003"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_median_blur_normalize_rotate.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="16"/>
+    <s v="Consolidation"/>
+    <n v="0.58073269999999999"/>
+    <n v="0.64102564100000003"/>
+    <n v="0.23636363599999999"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_median_blur_normalize_rotate.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="16"/>
+    <s v="Edema"/>
+    <n v="0.63885949399999997"/>
+    <n v="0.57264957299999997"/>
+    <n v="0.382716049"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_median_blur_normalize_rotate.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="16"/>
+    <s v="Pleural Effusion"/>
+    <n v="0.66341943000000003"/>
+    <n v="0.64957264999999997"/>
+    <n v="0.51190476200000001"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_rotate.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="17"/>
+    <s v="Atelectasis"/>
+    <n v="0.65413960999999998"/>
+    <n v="0.606837607"/>
+    <n v="0.53535353500000005"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_rotate.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="17"/>
+    <s v="Cardiomegaly"/>
+    <n v="0.73281360699999998"/>
+    <n v="0.73931623899999999"/>
+    <n v="0.57342657299999999"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_rotate.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="17"/>
+    <s v="Consolidation"/>
+    <n v="0.58269259799999995"/>
+    <n v="0.62820512799999995"/>
+    <n v="0.21621621599999999"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_rotate.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="17"/>
+    <s v="Edema"/>
+    <n v="0.65837742499999996"/>
+    <n v="0.56837606799999996"/>
+    <n v="0.38036809799999999"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_rotate.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="17"/>
+    <s v="Pleural Effusion"/>
+    <n v="0.66931808000000004"/>
+    <n v="0.62393162400000002"/>
+    <n v="0.51648351599999998"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_median_blur_rotate.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="18"/>
+    <s v="Atelectasis"/>
+    <n v="0.58831168831168801"/>
+    <n v="0.52136752136752096"/>
+    <n v="0.50442477876106195"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_median_blur_rotate.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="18"/>
+    <s v="Cardiomegaly"/>
+    <n v="0.67593905031892199"/>
+    <n v="0.61111111111111105"/>
+    <n v="0.51336898395721897"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_median_blur_rotate.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="18"/>
+    <s v="Consolidation"/>
+    <n v="0.67812452887079699"/>
+    <n v="0.61111111111111105"/>
+    <n v="0.33576642335766399"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_median_blur_rotate.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="18"/>
+    <s v="Edema"/>
+    <n v="0.67189888300999401"/>
+    <n v="0.59401709401709402"/>
+    <n v="0.41717791411042898"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_median_blur_rotate.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="18"/>
+    <s v="Pleural Effusion"/>
+    <n v="0.66301724908392101"/>
+    <n v="0.64957264957264904"/>
+    <n v="0.50602409638554202"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_median_blur_normalize_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="19"/>
+    <s v="Atelectasis"/>
+    <n v="0.67073863636363595"/>
+    <n v="0.61111111111111105"/>
+    <n v="0.538071065989847"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_median_blur_normalize_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="19"/>
+    <s v="Cardiomegaly"/>
+    <n v="0.71669029057406097"/>
+    <n v="0.72649572649572602"/>
+    <n v="0.55555555555555503"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_median_blur_normalize_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="19"/>
+    <s v="Consolidation"/>
+    <n v="0.62761947836574705"/>
+    <n v="0.68803418803418803"/>
+    <n v="0.29126213592233002"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_median_blur_normalize_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="19"/>
+    <s v="Edema"/>
+    <n v="0.65502645502645496"/>
+    <n v="0.63675213675213604"/>
+    <n v="0.388489208633093"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_median_blur_normalize_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="19"/>
+    <s v="Pleural Effusion"/>
+    <n v="0.65573330950040198"/>
+    <n v="0.62820512820512797"/>
+    <n v="0.46625766871165603"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_median_blur_normalize_rotate_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="20"/>
+    <s v="Atelectasis"/>
+    <n v="0.58104707792207699"/>
+    <n v="0.54273504273504203"/>
+    <n v="0.502325581395348"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_median_blur_normalize_rotate_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="20"/>
+    <s v="Cardiomegaly"/>
+    <n v="0.71695605953224595"/>
+    <n v="0.68803418803418803"/>
+    <n v="0.55214723926380305"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_median_blur_normalize_rotate_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="20"/>
+    <s v="Consolidation"/>
+    <n v="0.71046283732850901"/>
+    <n v="0.73076923076922995"/>
+    <n v="0.36363636363636298"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_median_blur_normalize_rotate_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="20"/>
+    <s v="Edema"/>
+    <n v="0.67677836566725402"/>
+    <n v="0.59829059829059805"/>
+    <n v="0.41249999999999998"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_median_blur_normalize_rotate_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="20"/>
+    <s v="Pleural Effusion"/>
+    <n v="0.64876217713826001"/>
+    <n v="0.62393162393162305"/>
+    <n v="0.49425287356321801"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="21"/>
+    <s v="Atelectasis"/>
+    <n v="0.64403409090909003"/>
+    <n v="0.58119658119658102"/>
+    <n v="0.51485148514851398"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="21"/>
+    <s v="Cardiomegaly"/>
+    <n v="0.70729978738483301"/>
+    <n v="0.66666666666666596"/>
+    <n v="0.51249999999999996"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="21"/>
+    <s v="Consolidation"/>
+    <n v="0.65551032715211799"/>
+    <n v="0.60256410256410198"/>
+    <n v="0.33093525179856098"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="21"/>
+    <s v="Edema"/>
+    <n v="0.638800705467372"/>
+    <n v="0.58974358974358898"/>
+    <n v="0.36"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="21"/>
+    <s v="Pleural Effusion"/>
+    <n v="0.67512735722584605"/>
+    <n v="0.658119658119658"/>
+    <n v="0.52941176470588203"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_rotate_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="22"/>
+    <s v="Atelectasis"/>
+    <n v="0.59241071428571401"/>
+    <n v="0.53418803418803396"/>
+    <n v="0.49302325581395301"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_rotate_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="22"/>
+    <s v="Cardiomegaly"/>
+    <n v="0.72293586109142405"/>
+    <n v="0.69230769230769196"/>
+    <n v="0.56097560975609695"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_rotate_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="22"/>
+    <s v="Consolidation"/>
+    <n v="0.65196743554952497"/>
+    <n v="0.69658119658119599"/>
+    <n v="0.28282828282828198"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_rotate_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="22"/>
+    <s v="Edema"/>
+    <n v="0.68812463256907697"/>
+    <n v="0.62393162393162305"/>
+    <n v="0.443037974683544"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_rotate_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="22"/>
+    <s v="Pleural Effusion"/>
+    <n v="0.64076324962016196"/>
+    <n v="0.60683760683760601"/>
+    <n v="0.47727272727272702"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_median_blur_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="23"/>
+    <s v="Atelectasis"/>
+    <n v="0.62637987012986995"/>
+    <n v="0.57264957264957195"/>
+    <n v="0.53271028037383095"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_median_blur_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="23"/>
+    <s v="Cardiomegaly"/>
+    <n v="0.704287739192062"/>
+    <n v="0.70512820512820495"/>
+    <n v="0.50359712230215803"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_median_blur_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="23"/>
+    <s v="Consolidation"/>
+    <n v="0.66289763304688598"/>
+    <n v="0.67521367521367504"/>
+    <n v="0.269230769230769"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_median_blur_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="23"/>
+    <s v="Edema"/>
+    <n v="0.66654908877131103"/>
+    <n v="0.58974358974358898"/>
+    <n v="0.407407407407407"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_median_blur_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="23"/>
+    <s v="Pleural Effusion"/>
+    <n v="0.682992224506211"/>
+    <n v="0.658119658119658"/>
+    <n v="0.52941176470588203"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_median_blur_rotate_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="24"/>
+    <s v="Atelectasis"/>
+    <n v="0.60677759740259696"/>
+    <n v="0.52564102564102499"/>
+    <n v="0.52360515021459197"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_median_blur_rotate_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="24"/>
+    <s v="Cardiomegaly"/>
+    <n v="0.70490786676116202"/>
+    <n v="0.67521367521367504"/>
+    <n v="0.530864197530864"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_median_blur_rotate_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="24"/>
+    <s v="Consolidation"/>
+    <n v="0.61435248002412102"/>
+    <n v="0.61111111111111105"/>
+    <n v="0.24793388429752"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_median_blur_rotate_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="24"/>
+    <s v="Edema"/>
+    <n v="0.63562610229276895"/>
+    <n v="0.55982905982905895"/>
+    <n v="0.36024844720496801"/>
+  </r>
+  <r>
+    <s v="Namespace(batchsize=32, file='image_preprocessing', limit=2048, map='Random', path='D:\\Uni\\Masters\\ISSS610 Applied Machine Learning\\Project\\chexpert-aml', pca=False, preprocessing='notebooks\\crop_eqhist_median_blur_rotate_zoom.yaml', ylabels=['Atelectasis', 'Cardiomegaly', 'Consolidation', 'Edema', 'Pleural Effusion'])"/>
+    <x v="24"/>
+    <s v="Pleural Effusion"/>
+    <n v="0.65475020109035598"/>
+    <n v="0.62393162393162305"/>
+    <n v="0.52688172043010695"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:D20" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <location ref="A3:D29" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="17">
+      <items count="26">
         <item x="5"/>
         <item x="13"/>
         <item x="4"/>
@@ -1574,12 +2091,21 @@
         <item x="15"/>
         <item x="6"/>
         <item x="14"/>
+        <item x="18"/>
+        <item x="24"/>
+        <item x="23"/>
         <item x="12"/>
+        <item x="17"/>
+        <item x="22"/>
+        <item x="21"/>
         <item x="0"/>
         <item x="3"/>
         <item x="11"/>
         <item x="2"/>
         <item x="10"/>
+        <item x="16"/>
+        <item x="20"/>
+        <item x="19"/>
         <item x="8"/>
         <item x="1"/>
         <item x="9"/>
@@ -1594,7 +2120,7 @@
   <rowFields count="1">
     <field x="1"/>
   </rowFields>
-  <rowItems count="17">
+  <rowItems count="26">
     <i>
       <x/>
     </i>
@@ -1643,6 +2169,33 @@
     <i>
       <x v="15"/>
     </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
     <i t="grand">
       <x/>
     </i>
@@ -1666,37 +2219,13 @@
     <dataField name="Average of accuracy" fld="4" subtotal="average" baseField="1" baseItem="0"/>
     <dataField name="Average of f1_score" fld="5" subtotal="average" baseField="1" baseItem="0"/>
   </dataFields>
-  <formats count="6">
-    <format dxfId="5">
+  <formats count="5">
+    <format dxfId="0">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="12"/>
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
           </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="4">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="12"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="3">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="2">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
           <reference field="1" count="1">
             <x v="5"/>
           </reference>
@@ -1705,18 +2234,48 @@
     </format>
     <format dxfId="1">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="18"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="2">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
           <reference field="1" count="1">
             <x v="2"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
+    <format dxfId="3">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
           <reference field="1" count="1">
-            <x v="2"/>
+            <x v="20"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="4">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="9"/>
           </reference>
         </references>
       </pivotArea>
@@ -2031,15 +2590,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D20"/>
+  <dimension ref="A3:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="76" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="85.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.88671875" bestFit="1" customWidth="1"/>
@@ -2047,16 +2606,16 @@
   <sheetData>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -2078,26 +2637,26 @@
         <v>38</v>
       </c>
       <c r="B5" s="3">
-        <v>0.41422487868814839</v>
+        <v>0.41422487859999996</v>
       </c>
       <c r="C5" s="3">
-        <v>0.70598290598290547</v>
+        <v>0.70598290600000002</v>
       </c>
       <c r="D5" s="3">
-        <v>5.1168786347830522E-2</v>
+        <v>5.1168786200000003E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>0.68214787780000008</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="3">
         <v>0.66068376060000011</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="3">
         <v>0.4869916313999999</v>
       </c>
     </row>
@@ -2120,26 +2679,26 @@
         <v>42</v>
       </c>
       <c r="B8" s="3">
-        <v>0.41809718057821543</v>
+        <v>0.41809718060000006</v>
       </c>
       <c r="C8" s="3">
-        <v>0.70769230769230718</v>
+        <v>0.70769230760000001</v>
       </c>
       <c r="D8" s="3">
-        <v>3.1505558696061781E-2</v>
+        <v>3.1505558599999997E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>0.6827887722</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="3">
         <v>0.62991452979999996</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="3">
         <v>0.47301936239999998</v>
       </c>
     </row>
@@ -2148,153 +2707,279 @@
         <v>40</v>
       </c>
       <c r="B10" s="3">
-        <v>0.41170483228289462</v>
+        <v>0.41170483220000004</v>
       </c>
       <c r="C10" s="3">
-        <v>0.71111111111111036</v>
+        <v>0.71111111119999992</v>
       </c>
       <c r="D10" s="3">
-        <v>3.1937984496123999E-2</v>
+        <v>3.1937984600000004E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B11" s="3">
-        <v>0.42990706550469093</v>
+        <v>0.65545827991906447</v>
       </c>
       <c r="C11" s="3">
-        <v>0.70683760683760632</v>
+        <v>0.59743589743589731</v>
       </c>
       <c r="D11" s="3">
-        <v>4.679896462467624E-2</v>
+        <v>0.45535243931438318</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="B12" s="3">
-        <v>0.6091885292</v>
+        <v>0.64328284951420101</v>
       </c>
       <c r="C12" s="3">
-        <v>0.62393162400000002</v>
+        <v>0.59914529914529868</v>
       </c>
       <c r="D12" s="3">
-        <v>0.43087332900000003</v>
+        <v>0.43790667993561022</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="3">
-        <v>0.65510993740000001</v>
+        <v>58</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0.66862131112926804</v>
       </c>
       <c r="C13" s="3">
-        <v>0.62649572659999986</v>
+        <v>0.64017094017093978</v>
       </c>
       <c r="D13" s="3">
-        <v>0.44647752480000003</v>
+        <v>0.44847146880400934</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B14" s="3">
-        <v>0.42981924190015164</v>
+        <v>0.42990706539999995</v>
       </c>
       <c r="C14" s="3">
-        <v>0.71538461538461473</v>
+        <v>0.70683760679999996</v>
       </c>
       <c r="D14" s="3">
-        <v>4.4807596201898982E-2</v>
+        <v>4.67989646E-2</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="B15" s="3">
-        <v>0.60986682240000001</v>
+        <v>0.65946826399999992</v>
       </c>
       <c r="C15" s="3">
-        <v>0.59658119640000007</v>
+        <v>0.63333333319999996</v>
       </c>
       <c r="D15" s="3">
-        <v>0.43026660820000001</v>
+        <v>0.44436958759999995</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="5">
-        <v>0.68808467989228095</v>
-      </c>
-      <c r="C16" s="5">
-        <v>0.64358974358974286</v>
-      </c>
-      <c r="D16" s="5">
-        <v>0.47118776462090806</v>
+      <c r="A16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0.65924037862318041</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.63076923076923019</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.4514275700709206</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="B17" s="3">
-        <v>0.66182983665386907</v>
+        <v>0.66415445362785186</v>
       </c>
       <c r="C17" s="3">
-        <v>0.63333333333333286</v>
+        <v>0.61965811965811912</v>
       </c>
       <c r="D17" s="3">
-        <v>0.45400018660133645</v>
+        <v>0.44953970033059143</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B18" s="3">
-        <v>0.6563855408</v>
+        <v>0.6091885292</v>
       </c>
       <c r="C18" s="3">
-        <v>0.63760683759999992</v>
+        <v>0.62393162400000002</v>
       </c>
       <c r="D18" s="3">
-        <v>0.45682161040000002</v>
+        <v>0.43087332900000003</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B19" s="3">
-        <v>0.42807062954996378</v>
+        <v>0.65510993740000001</v>
       </c>
       <c r="C19" s="3">
-        <v>0.71282051282051229</v>
+        <v>0.62649572659999986</v>
       </c>
       <c r="D19" s="3">
-        <v>2.6044845291036123E-2</v>
+        <v>0.44647752480000003</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0.42981924180000008</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.71538461539999998</v>
+      </c>
+      <c r="D20" s="3">
+        <v>4.4807595999999998E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="3">
+        <v>0.60986682240000001</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.59658119640000007</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0.43026660820000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="4">
+        <v>0.68808468</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.6435897436000001</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.47118776460000006</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="3">
-        <v>0.56624091375313856</v>
-      </c>
-      <c r="C20" s="3">
-        <v>0.6588675213345081</v>
-      </c>
-      <c r="D20" s="3">
-        <v>0.29438383946749203</v>
+      <c r="B23" s="3">
+        <v>0.63367945300000006</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.61367521380000001</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0.42180987199999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="5">
+        <v>0.6668013035176692</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.63675213675213616</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0.4649724115717464</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0.66516163396606021</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0.65811965811965778</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0.4479271269624962</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="3">
+        <v>0.66182983660000005</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0.63333333340000009</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0.45400018639999995</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0.6563855408</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0.63760683759999992</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0.45682161040000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0.42807062959999997</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0.71282051280000003</v>
+      </c>
+      <c r="D28" s="3">
+        <v>2.6044845399999999E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="3">
+        <v>0.59902890188389168</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0.64683760681805158</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0.34927673150359029</v>
       </c>
     </row>
   </sheetData>
@@ -2304,10 +2989,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:F126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3143,13 +3828,13 @@
         <v>8</v>
       </c>
       <c r="D42">
-        <v>0.63457792207792196</v>
+        <v>0.63457792199999996</v>
       </c>
       <c r="E42">
-        <v>0.59401709401709402</v>
+        <v>0.59401709400000002</v>
       </c>
       <c r="F42">
-        <v>0.53658536585365801</v>
+        <v>0.53658536599999995</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -3163,10 +3848,10 @@
         <v>9</v>
       </c>
       <c r="D43">
-        <v>0.71305811481218995</v>
+        <v>0.71305811500000005</v>
       </c>
       <c r="E43">
-        <v>0.683760683760683</v>
+        <v>0.68376068400000001</v>
       </c>
       <c r="F43">
         <v>0.53749999999999998</v>
@@ -3183,13 +3868,13 @@
         <v>10</v>
       </c>
       <c r="D44">
-        <v>0.64601236243027205</v>
+        <v>0.64601236200000001</v>
       </c>
       <c r="E44">
-        <v>0.69230769230769196</v>
+        <v>0.69230769199999997</v>
       </c>
       <c r="F44">
-        <v>0.33333333333333298</v>
+        <v>0.33333333300000001</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -3203,13 +3888,13 @@
         <v>11</v>
       </c>
       <c r="D45">
-        <v>0.65802469135802399</v>
+        <v>0.65802469100000005</v>
       </c>
       <c r="E45">
-        <v>0.55982905982905895</v>
+        <v>0.55982905999999999</v>
       </c>
       <c r="F45">
-        <v>0.390532544378698</v>
+        <v>0.39053254399999998</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -3223,13 +3908,13 @@
         <v>12</v>
       </c>
       <c r="D46">
-        <v>0.65747609259093698</v>
+        <v>0.65747609299999998</v>
       </c>
       <c r="E46">
-        <v>0.63675213675213604</v>
+        <v>0.636752137</v>
       </c>
       <c r="F46">
-        <v>0.47204968944099301</v>
+        <v>0.47204968899999999</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -3243,10 +3928,10 @@
         <v>8</v>
       </c>
       <c r="D47">
-        <v>0.34537337662337603</v>
+        <v>0.34537337699999998</v>
       </c>
       <c r="E47">
-        <v>0.61111111111111105</v>
+        <v>0.61111111100000004</v>
       </c>
       <c r="F47">
         <v>0</v>
@@ -3263,13 +3948,13 @@
         <v>9</v>
       </c>
       <c r="D48">
-        <v>0.42762225372076501</v>
+        <v>0.42762225399999998</v>
       </c>
       <c r="E48">
-        <v>0.67948717948717896</v>
+        <v>0.679487179</v>
       </c>
       <c r="F48">
-        <v>2.5974025974025899E-2</v>
+        <v>2.5974026000000001E-2</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -3283,10 +3968,10 @@
         <v>10</v>
       </c>
       <c r="D49">
-        <v>0.41579978893411701</v>
+        <v>0.41579978899999998</v>
       </c>
       <c r="E49">
-        <v>0.854700854700854</v>
+        <v>0.85470085500000004</v>
       </c>
       <c r="F49">
         <v>0</v>
@@ -3303,13 +3988,13 @@
         <v>11</v>
       </c>
       <c r="D50">
-        <v>0.452674897119341</v>
+        <v>0.45267489700000002</v>
       </c>
       <c r="E50">
-        <v>0.76068376068375998</v>
+        <v>0.76068376100000001</v>
       </c>
       <c r="F50">
-        <v>3.4482758620689599E-2</v>
+        <v>3.4482759000000002E-2</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -3323,13 +4008,13 @@
         <v>12</v>
       </c>
       <c r="D51">
-        <v>0.49888283135222</v>
+        <v>0.49888283100000003</v>
       </c>
       <c r="E51">
-        <v>0.658119658119658</v>
+        <v>0.65811965800000005</v>
       </c>
       <c r="F51">
-        <v>6.9767441860465101E-2</v>
+        <v>6.9767441999999999E-2</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -3343,13 +4028,13 @@
         <v>8</v>
       </c>
       <c r="D52">
-        <v>0.63835227272727202</v>
+        <v>0.63835227299999997</v>
       </c>
       <c r="E52">
-        <v>0.60256410256410198</v>
+        <v>0.60256410299999996</v>
       </c>
       <c r="F52">
-        <v>0.53266331658291399</v>
+        <v>0.53266331700000003</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -3363,10 +4048,10 @@
         <v>9</v>
       </c>
       <c r="D53">
-        <v>0.73175053153791603</v>
+        <v>0.73175053199999995</v>
       </c>
       <c r="E53">
-        <v>0.70085470085470003</v>
+        <v>0.70085470100000002</v>
       </c>
       <c r="F53">
         <v>0.5625</v>
@@ -3383,13 +4068,13 @@
         <v>10</v>
       </c>
       <c r="D54">
-        <v>0.71702095582692604</v>
+        <v>0.71702095600000004</v>
       </c>
       <c r="E54">
-        <v>0.67948717948717896</v>
+        <v>0.679487179</v>
       </c>
       <c r="F54">
-        <v>0.369747899159663</v>
+        <v>0.36974789899999999</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -3403,10 +4088,10 @@
         <v>11</v>
       </c>
       <c r="D55">
-        <v>0.68165784832451504</v>
+        <v>0.68165784799999996</v>
       </c>
       <c r="E55">
-        <v>0.59829059829059805</v>
+        <v>0.59829059799999995</v>
       </c>
       <c r="F55">
         <v>0.41249999999999998</v>
@@ -3423,13 +4108,13 @@
         <v>12</v>
       </c>
       <c r="D56">
-        <v>0.67164179104477595</v>
+        <v>0.67164179099999999</v>
       </c>
       <c r="E56">
-        <v>0.63675213675213604</v>
+        <v>0.636752137</v>
       </c>
       <c r="F56">
-        <v>0.47852760736196298</v>
+        <v>0.47852760700000002</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -3443,13 +4128,13 @@
         <v>8</v>
       </c>
       <c r="D57">
-        <v>0.34082792207792201</v>
+        <v>0.34082792200000001</v>
       </c>
       <c r="E57">
-        <v>0.61538461538461497</v>
+        <v>0.61538461499999997</v>
       </c>
       <c r="F57">
-        <v>2.1739130434782601E-2</v>
+        <v>2.1739129999999999E-2</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -3463,10 +4148,10 @@
         <v>9</v>
       </c>
       <c r="D58">
-        <v>0.43320340184266398</v>
+        <v>0.43320340200000002</v>
       </c>
       <c r="E58">
-        <v>0.67521367521367504</v>
+        <v>0.67521367499999996</v>
       </c>
       <c r="F58">
         <v>0</v>
@@ -3483,10 +4168,10 @@
         <v>10</v>
       </c>
       <c r="D59">
-        <v>0.42740841248303901</v>
+        <v>0.42740841200000002</v>
       </c>
       <c r="E59">
-        <v>0.854700854700854</v>
+        <v>0.85470085500000004</v>
       </c>
       <c r="F59">
         <v>0</v>
@@ -3503,13 +4188,13 @@
         <v>11</v>
       </c>
       <c r="D60">
-        <v>0.463609641387419</v>
+        <v>0.46360964100000002</v>
       </c>
       <c r="E60">
-        <v>0.77777777777777701</v>
+        <v>0.77777777800000003</v>
       </c>
       <c r="F60">
-        <v>0.133333333333333</v>
+        <v>0.133333333</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -3523,13 +4208,13 @@
         <v>12</v>
       </c>
       <c r="D61">
-        <v>0.48404683170971402</v>
+        <v>0.48404683199999998</v>
       </c>
       <c r="E61">
-        <v>0.65384615384615297</v>
+        <v>0.65384615400000001</v>
       </c>
       <c r="F61">
-        <v>6.8965517241379296E-2</v>
+        <v>6.8965517000000004E-2</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -3543,10 +4228,10 @@
         <v>8</v>
       </c>
       <c r="D62">
-        <v>0.32694805194805199</v>
+        <v>0.32694805199999999</v>
       </c>
       <c r="E62">
-        <v>0.60683760683760601</v>
+        <v>0.606837607</v>
       </c>
       <c r="F62">
         <v>0</v>
@@ -3563,10 +4248,10 @@
         <v>9</v>
       </c>
       <c r="D63">
-        <v>0.41087880935506699</v>
+        <v>0.41087880900000001</v>
       </c>
       <c r="E63">
-        <v>0.66666666666666596</v>
+        <v>0.66666666699999999</v>
       </c>
       <c r="F63">
         <v>0</v>
@@ -3583,10 +4268,10 @@
         <v>10</v>
       </c>
       <c r="D64">
-        <v>0.40524649479873298</v>
+        <v>0.40524649499999998</v>
       </c>
       <c r="E64">
-        <v>0.841880341880341</v>
+        <v>0.84188034199999995</v>
       </c>
       <c r="F64">
         <v>0</v>
@@ -3603,13 +4288,13 @@
         <v>11</v>
       </c>
       <c r="D65">
-        <v>0.44832451499118098</v>
+        <v>0.44832451499999998</v>
       </c>
       <c r="E65">
-        <v>0.75641025641025605</v>
+        <v>0.756410256</v>
       </c>
       <c r="F65">
-        <v>6.5573770491803199E-2</v>
+        <v>6.5573770000000003E-2</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -3623,13 +4308,13 @@
         <v>12</v>
       </c>
       <c r="D66">
-        <v>0.55813745643042201</v>
+        <v>0.55813745599999998</v>
       </c>
       <c r="E66">
-        <v>0.66239316239316204</v>
+        <v>0.66239316199999998</v>
       </c>
       <c r="F66">
-        <v>0.168421052631578</v>
+        <v>0.16842105299999999</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -3643,13 +4328,13 @@
         <v>8</v>
       </c>
       <c r="D67">
-        <v>0.36899350649350598</v>
+        <v>0.36899350600000003</v>
       </c>
       <c r="E67">
-        <v>0.60256410256410198</v>
+        <v>0.60256410299999996</v>
       </c>
       <c r="F67">
-        <v>4.1237113402061799E-2</v>
+        <v>4.1237112999999999E-2</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -3663,13 +4348,13 @@
         <v>9</v>
       </c>
       <c r="D68">
-        <v>0.43594968107725002</v>
+        <v>0.43594968099999998</v>
       </c>
       <c r="E68">
-        <v>0.66666666666666596</v>
+        <v>0.66666666699999999</v>
       </c>
       <c r="F68">
-        <v>4.8780487804878002E-2</v>
+        <v>4.8780487999999997E-2</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -3683,10 +4368,10 @@
         <v>10</v>
       </c>
       <c r="D69">
-        <v>0.42921754862053302</v>
+        <v>0.42921754899999998</v>
       </c>
       <c r="E69">
-        <v>0.841880341880341</v>
+        <v>0.84188034199999995</v>
       </c>
       <c r="F69">
         <v>0</v>
@@ -3703,13 +4388,13 @@
         <v>11</v>
       </c>
       <c r="D70">
-        <v>0.44291593180481997</v>
+        <v>0.44291593200000001</v>
       </c>
       <c r="E70">
-        <v>0.75641025641025605</v>
+        <v>0.756410256</v>
       </c>
       <c r="F70">
-        <v>9.5238095238095205E-2</v>
+        <v>9.5238094999999995E-2</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -3723,13 +4408,13 @@
         <v>12</v>
       </c>
       <c r="D71">
-        <v>0.39404772544463301</v>
+        <v>0.39404772500000002</v>
       </c>
       <c r="E71">
-        <v>0.66239316239316204</v>
+        <v>0.66239316199999998</v>
       </c>
       <c r="F71">
-        <v>7.0588235294117604E-2</v>
+        <v>7.0588234999999999E-2</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -3743,10 +4428,10 @@
         <v>8</v>
       </c>
       <c r="D72">
-        <v>0.32930194805194801</v>
+        <v>0.32930194800000001</v>
       </c>
       <c r="E72">
-        <v>0.60683760683760601</v>
+        <v>0.606837607</v>
       </c>
       <c r="F72">
         <v>0</v>
@@ -3763,10 +4448,10 @@
         <v>9</v>
       </c>
       <c r="D73">
-        <v>0.40786676116229598</v>
+        <v>0.40786676100000002</v>
       </c>
       <c r="E73">
-        <v>0.67948717948717896</v>
+        <v>0.679487179</v>
       </c>
       <c r="F73">
         <v>0</v>
@@ -3783,10 +4468,10 @@
         <v>10</v>
       </c>
       <c r="D74">
-        <v>0.40419116538519501</v>
+        <v>0.40419116500000002</v>
       </c>
       <c r="E74">
-        <v>0.841880341880341</v>
+        <v>0.84188034199999995</v>
       </c>
       <c r="F74">
         <v>0</v>
@@ -3803,13 +4488,13 @@
         <v>11</v>
       </c>
       <c r="D75">
-        <v>0.444914756025867</v>
+        <v>0.44491475600000002</v>
       </c>
       <c r="E75">
-        <v>0.76068376068375998</v>
+        <v>0.76068376100000001</v>
       </c>
       <c r="F75">
-        <v>6.6666666666666596E-2</v>
+        <v>6.6666666999999999E-2</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -3823,13 +4508,13 @@
         <v>12</v>
       </c>
       <c r="D76">
-        <v>0.47224953078916698</v>
+        <v>0.472249531</v>
       </c>
       <c r="E76">
-        <v>0.66666666666666596</v>
+        <v>0.66666666699999999</v>
       </c>
       <c r="F76">
-        <v>9.3023255813953404E-2</v>
+        <v>9.3023255999999999E-2</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -3843,10 +4528,10 @@
         <v>8</v>
       </c>
       <c r="D77">
-        <v>0.32646103896103901</v>
+        <v>0.32646103900000001</v>
       </c>
       <c r="E77">
-        <v>0.61111111111111105</v>
+        <v>0.61111111100000004</v>
       </c>
       <c r="F77">
         <v>0</v>
@@ -3863,10 +4548,10 @@
         <v>9</v>
       </c>
       <c r="D78">
-        <v>0.41123316796598097</v>
+        <v>0.41123316799999998</v>
       </c>
       <c r="E78">
-        <v>0.67094017094017</v>
+        <v>0.67094017100000003</v>
       </c>
       <c r="F78">
         <v>0</v>
@@ -3883,10 +4568,10 @@
         <v>10</v>
       </c>
       <c r="D79">
-        <v>0.40434192672998598</v>
+        <v>0.40434192699999999</v>
       </c>
       <c r="E79">
-        <v>0.83760683760683696</v>
+        <v>0.83760683800000002</v>
       </c>
       <c r="F79">
         <v>0</v>
@@ -3903,13 +4588,13 @@
         <v>11</v>
       </c>
       <c r="D80">
-        <v>0.44456202233980002</v>
+        <v>0.444562022</v>
       </c>
       <c r="E80">
-        <v>0.75641025641025605</v>
+        <v>0.756410256</v>
       </c>
       <c r="F80">
-        <v>6.5573770491803199E-2</v>
+        <v>6.5573770000000003E-2</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -3923,13 +4608,913 @@
         <v>12</v>
       </c>
       <c r="D81">
-        <v>0.50388774689427096</v>
+        <v>0.50388774700000005</v>
       </c>
       <c r="E81">
-        <v>0.66239316239316204</v>
+        <v>0.66239316199999998</v>
       </c>
       <c r="F81">
-        <v>9.1954022988505704E-2</v>
+        <v>9.1954022999999996E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>43</v>
+      </c>
+      <c r="B82" t="s">
+        <v>44</v>
+      </c>
+      <c r="C82" t="s">
+        <v>8</v>
+      </c>
+      <c r="D82">
+        <v>0.59066558400000002</v>
+      </c>
+      <c r="E82">
+        <v>0.54273504299999997</v>
+      </c>
+      <c r="F82">
+        <v>0.45685279200000001</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>43</v>
+      </c>
+      <c r="B83" t="s">
+        <v>44</v>
+      </c>
+      <c r="C83" t="s">
+        <v>9</v>
+      </c>
+      <c r="D83">
+        <v>0.69472005699999995</v>
+      </c>
+      <c r="E83">
+        <v>0.66239316199999998</v>
+      </c>
+      <c r="F83">
+        <v>0.52121212100000003</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>43</v>
+      </c>
+      <c r="B84" t="s">
+        <v>44</v>
+      </c>
+      <c r="C84" t="s">
+        <v>10</v>
+      </c>
+      <c r="D84">
+        <v>0.58073269999999999</v>
+      </c>
+      <c r="E84">
+        <v>0.64102564100000003</v>
+      </c>
+      <c r="F84">
+        <v>0.23636363599999999</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>43</v>
+      </c>
+      <c r="B85" t="s">
+        <v>44</v>
+      </c>
+      <c r="C85" t="s">
+        <v>11</v>
+      </c>
+      <c r="D85">
+        <v>0.63885949399999997</v>
+      </c>
+      <c r="E85">
+        <v>0.57264957299999997</v>
+      </c>
+      <c r="F85">
+        <v>0.382716049</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>43</v>
+      </c>
+      <c r="B86" t="s">
+        <v>44</v>
+      </c>
+      <c r="C86" t="s">
+        <v>12</v>
+      </c>
+      <c r="D86">
+        <v>0.66341943000000003</v>
+      </c>
+      <c r="E86">
+        <v>0.64957264999999997</v>
+      </c>
+      <c r="F86">
+        <v>0.51190476200000001</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>45</v>
+      </c>
+      <c r="B87" t="s">
+        <v>46</v>
+      </c>
+      <c r="C87" t="s">
+        <v>8</v>
+      </c>
+      <c r="D87">
+        <v>0.65413960999999998</v>
+      </c>
+      <c r="E87">
+        <v>0.606837607</v>
+      </c>
+      <c r="F87">
+        <v>0.53535353500000005</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>45</v>
+      </c>
+      <c r="B88" t="s">
+        <v>46</v>
+      </c>
+      <c r="C88" t="s">
+        <v>9</v>
+      </c>
+      <c r="D88">
+        <v>0.73281360699999998</v>
+      </c>
+      <c r="E88">
+        <v>0.73931623899999999</v>
+      </c>
+      <c r="F88">
+        <v>0.57342657299999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>45</v>
+      </c>
+      <c r="B89" t="s">
+        <v>46</v>
+      </c>
+      <c r="C89" t="s">
+        <v>10</v>
+      </c>
+      <c r="D89">
+        <v>0.58269259799999995</v>
+      </c>
+      <c r="E89">
+        <v>0.62820512799999995</v>
+      </c>
+      <c r="F89">
+        <v>0.21621621599999999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>45</v>
+      </c>
+      <c r="B90" t="s">
+        <v>46</v>
+      </c>
+      <c r="C90" t="s">
+        <v>11</v>
+      </c>
+      <c r="D90">
+        <v>0.65837742499999996</v>
+      </c>
+      <c r="E90">
+        <v>0.56837606799999996</v>
+      </c>
+      <c r="F90">
+        <v>0.38036809799999999</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>45</v>
+      </c>
+      <c r="B91" t="s">
+        <v>46</v>
+      </c>
+      <c r="C91" t="s">
+        <v>12</v>
+      </c>
+      <c r="D91">
+        <v>0.66931808000000004</v>
+      </c>
+      <c r="E91">
+        <v>0.62393162400000002</v>
+      </c>
+      <c r="F91">
+        <v>0.51648351599999998</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>47</v>
+      </c>
+      <c r="B92" t="s">
+        <v>48</v>
+      </c>
+      <c r="C92" t="s">
+        <v>8</v>
+      </c>
+      <c r="D92">
+        <v>0.58831168831168801</v>
+      </c>
+      <c r="E92">
+        <v>0.52136752136752096</v>
+      </c>
+      <c r="F92">
+        <v>0.50442477876106195</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>47</v>
+      </c>
+      <c r="B93" t="s">
+        <v>48</v>
+      </c>
+      <c r="C93" t="s">
+        <v>9</v>
+      </c>
+      <c r="D93">
+        <v>0.67593905031892199</v>
+      </c>
+      <c r="E93">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="F93">
+        <v>0.51336898395721897</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>47</v>
+      </c>
+      <c r="B94" t="s">
+        <v>48</v>
+      </c>
+      <c r="C94" t="s">
+        <v>10</v>
+      </c>
+      <c r="D94">
+        <v>0.67812452887079699</v>
+      </c>
+      <c r="E94">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="F94">
+        <v>0.33576642335766399</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>47</v>
+      </c>
+      <c r="B95" t="s">
+        <v>48</v>
+      </c>
+      <c r="C95" t="s">
+        <v>11</v>
+      </c>
+      <c r="D95">
+        <v>0.67189888300999401</v>
+      </c>
+      <c r="E95">
+        <v>0.59401709401709402</v>
+      </c>
+      <c r="F95">
+        <v>0.41717791411042898</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>47</v>
+      </c>
+      <c r="B96" t="s">
+        <v>48</v>
+      </c>
+      <c r="C96" t="s">
+        <v>12</v>
+      </c>
+      <c r="D96">
+        <v>0.66301724908392101</v>
+      </c>
+      <c r="E96">
+        <v>0.64957264957264904</v>
+      </c>
+      <c r="F96">
+        <v>0.50602409638554202</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>49</v>
+      </c>
+      <c r="B97" t="s">
+        <v>50</v>
+      </c>
+      <c r="C97" t="s">
+        <v>8</v>
+      </c>
+      <c r="D97">
+        <v>0.67073863636363595</v>
+      </c>
+      <c r="E97">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="F97">
+        <v>0.538071065989847</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>49</v>
+      </c>
+      <c r="B98" t="s">
+        <v>50</v>
+      </c>
+      <c r="C98" t="s">
+        <v>9</v>
+      </c>
+      <c r="D98">
+        <v>0.71669029057406097</v>
+      </c>
+      <c r="E98">
+        <v>0.72649572649572602</v>
+      </c>
+      <c r="F98">
+        <v>0.55555555555555503</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>49</v>
+      </c>
+      <c r="B99" t="s">
+        <v>50</v>
+      </c>
+      <c r="C99" t="s">
+        <v>10</v>
+      </c>
+      <c r="D99">
+        <v>0.62761947836574705</v>
+      </c>
+      <c r="E99">
+        <v>0.68803418803418803</v>
+      </c>
+      <c r="F99">
+        <v>0.29126213592233002</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>49</v>
+      </c>
+      <c r="B100" t="s">
+        <v>50</v>
+      </c>
+      <c r="C100" t="s">
+        <v>11</v>
+      </c>
+      <c r="D100">
+        <v>0.65502645502645496</v>
+      </c>
+      <c r="E100">
+        <v>0.63675213675213604</v>
+      </c>
+      <c r="F100">
+        <v>0.388489208633093</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>49</v>
+      </c>
+      <c r="B101" t="s">
+        <v>50</v>
+      </c>
+      <c r="C101" t="s">
+        <v>12</v>
+      </c>
+      <c r="D101">
+        <v>0.65573330950040198</v>
+      </c>
+      <c r="E101">
+        <v>0.62820512820512797</v>
+      </c>
+      <c r="F101">
+        <v>0.46625766871165603</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>51</v>
+      </c>
+      <c r="B102" t="s">
+        <v>52</v>
+      </c>
+      <c r="C102" t="s">
+        <v>8</v>
+      </c>
+      <c r="D102">
+        <v>0.58104707792207699</v>
+      </c>
+      <c r="E102">
+        <v>0.54273504273504203</v>
+      </c>
+      <c r="F102">
+        <v>0.502325581395348</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>51</v>
+      </c>
+      <c r="B103" t="s">
+        <v>52</v>
+      </c>
+      <c r="C103" t="s">
+        <v>9</v>
+      </c>
+      <c r="D103">
+        <v>0.71695605953224595</v>
+      </c>
+      <c r="E103">
+        <v>0.68803418803418803</v>
+      </c>
+      <c r="F103">
+        <v>0.55214723926380305</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>51</v>
+      </c>
+      <c r="B104" t="s">
+        <v>52</v>
+      </c>
+      <c r="C104" t="s">
+        <v>10</v>
+      </c>
+      <c r="D104">
+        <v>0.71046283732850901</v>
+      </c>
+      <c r="E104">
+        <v>0.73076923076922995</v>
+      </c>
+      <c r="F104">
+        <v>0.36363636363636298</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>51</v>
+      </c>
+      <c r="B105" t="s">
+        <v>52</v>
+      </c>
+      <c r="C105" t="s">
+        <v>11</v>
+      </c>
+      <c r="D105">
+        <v>0.67677836566725402</v>
+      </c>
+      <c r="E105">
+        <v>0.59829059829059805</v>
+      </c>
+      <c r="F105">
+        <v>0.41249999999999998</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>51</v>
+      </c>
+      <c r="B106" t="s">
+        <v>52</v>
+      </c>
+      <c r="C106" t="s">
+        <v>12</v>
+      </c>
+      <c r="D106">
+        <v>0.64876217713826001</v>
+      </c>
+      <c r="E106">
+        <v>0.62393162393162305</v>
+      </c>
+      <c r="F106">
+        <v>0.49425287356321801</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>53</v>
+      </c>
+      <c r="B107" t="s">
+        <v>54</v>
+      </c>
+      <c r="C107" t="s">
+        <v>8</v>
+      </c>
+      <c r="D107">
+        <v>0.64403409090909003</v>
+      </c>
+      <c r="E107">
+        <v>0.58119658119658102</v>
+      </c>
+      <c r="F107">
+        <v>0.51485148514851398</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>53</v>
+      </c>
+      <c r="B108" t="s">
+        <v>54</v>
+      </c>
+      <c r="C108" t="s">
+        <v>9</v>
+      </c>
+      <c r="D108">
+        <v>0.70729978738483301</v>
+      </c>
+      <c r="E108">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="F108">
+        <v>0.51249999999999996</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>53</v>
+      </c>
+      <c r="B109" t="s">
+        <v>54</v>
+      </c>
+      <c r="C109" t="s">
+        <v>10</v>
+      </c>
+      <c r="D109">
+        <v>0.65551032715211799</v>
+      </c>
+      <c r="E109">
+        <v>0.60256410256410198</v>
+      </c>
+      <c r="F109">
+        <v>0.33093525179856098</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>53</v>
+      </c>
+      <c r="B110" t="s">
+        <v>54</v>
+      </c>
+      <c r="C110" t="s">
+        <v>11</v>
+      </c>
+      <c r="D110">
+        <v>0.638800705467372</v>
+      </c>
+      <c r="E110">
+        <v>0.58974358974358898</v>
+      </c>
+      <c r="F110">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>53</v>
+      </c>
+      <c r="B111" t="s">
+        <v>54</v>
+      </c>
+      <c r="C111" t="s">
+        <v>12</v>
+      </c>
+      <c r="D111">
+        <v>0.67512735722584605</v>
+      </c>
+      <c r="E111">
+        <v>0.658119658119658</v>
+      </c>
+      <c r="F111">
+        <v>0.52941176470588203</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>55</v>
+      </c>
+      <c r="B112" t="s">
+        <v>56</v>
+      </c>
+      <c r="C112" t="s">
+        <v>8</v>
+      </c>
+      <c r="D112">
+        <v>0.59241071428571401</v>
+      </c>
+      <c r="E112">
+        <v>0.53418803418803396</v>
+      </c>
+      <c r="F112">
+        <v>0.49302325581395301</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>55</v>
+      </c>
+      <c r="B113" t="s">
+        <v>56</v>
+      </c>
+      <c r="C113" t="s">
+        <v>9</v>
+      </c>
+      <c r="D113">
+        <v>0.72293586109142405</v>
+      </c>
+      <c r="E113">
+        <v>0.69230769230769196</v>
+      </c>
+      <c r="F113">
+        <v>0.56097560975609695</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>55</v>
+      </c>
+      <c r="B114" t="s">
+        <v>56</v>
+      </c>
+      <c r="C114" t="s">
+        <v>10</v>
+      </c>
+      <c r="D114">
+        <v>0.65196743554952497</v>
+      </c>
+      <c r="E114">
+        <v>0.69658119658119599</v>
+      </c>
+      <c r="F114">
+        <v>0.28282828282828198</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>55</v>
+      </c>
+      <c r="B115" t="s">
+        <v>56</v>
+      </c>
+      <c r="C115" t="s">
+        <v>11</v>
+      </c>
+      <c r="D115">
+        <v>0.68812463256907697</v>
+      </c>
+      <c r="E115">
+        <v>0.62393162393162305</v>
+      </c>
+      <c r="F115">
+        <v>0.443037974683544</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>55</v>
+      </c>
+      <c r="B116" t="s">
+        <v>56</v>
+      </c>
+      <c r="C116" t="s">
+        <v>12</v>
+      </c>
+      <c r="D116">
+        <v>0.64076324962016196</v>
+      </c>
+      <c r="E116">
+        <v>0.60683760683760601</v>
+      </c>
+      <c r="F116">
+        <v>0.47727272727272702</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>57</v>
+      </c>
+      <c r="B117" t="s">
+        <v>58</v>
+      </c>
+      <c r="C117" t="s">
+        <v>8</v>
+      </c>
+      <c r="D117">
+        <v>0.62637987012986995</v>
+      </c>
+      <c r="E117">
+        <v>0.57264957264957195</v>
+      </c>
+      <c r="F117">
+        <v>0.53271028037383095</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>57</v>
+      </c>
+      <c r="B118" t="s">
+        <v>58</v>
+      </c>
+      <c r="C118" t="s">
+        <v>9</v>
+      </c>
+      <c r="D118">
+        <v>0.704287739192062</v>
+      </c>
+      <c r="E118">
+        <v>0.70512820512820495</v>
+      </c>
+      <c r="F118">
+        <v>0.50359712230215803</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>57</v>
+      </c>
+      <c r="B119" t="s">
+        <v>58</v>
+      </c>
+      <c r="C119" t="s">
+        <v>10</v>
+      </c>
+      <c r="D119">
+        <v>0.66289763304688598</v>
+      </c>
+      <c r="E119">
+        <v>0.67521367521367504</v>
+      </c>
+      <c r="F119">
+        <v>0.269230769230769</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>57</v>
+      </c>
+      <c r="B120" t="s">
+        <v>58</v>
+      </c>
+      <c r="C120" t="s">
+        <v>11</v>
+      </c>
+      <c r="D120">
+        <v>0.66654908877131103</v>
+      </c>
+      <c r="E120">
+        <v>0.58974358974358898</v>
+      </c>
+      <c r="F120">
+        <v>0.407407407407407</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>57</v>
+      </c>
+      <c r="B121" t="s">
+        <v>58</v>
+      </c>
+      <c r="C121" t="s">
+        <v>12</v>
+      </c>
+      <c r="D121">
+        <v>0.682992224506211</v>
+      </c>
+      <c r="E121">
+        <v>0.658119658119658</v>
+      </c>
+      <c r="F121">
+        <v>0.52941176470588203</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>59</v>
+      </c>
+      <c r="B122" t="s">
+        <v>60</v>
+      </c>
+      <c r="C122" t="s">
+        <v>8</v>
+      </c>
+      <c r="D122">
+        <v>0.60677759740259696</v>
+      </c>
+      <c r="E122">
+        <v>0.52564102564102499</v>
+      </c>
+      <c r="F122">
+        <v>0.52360515021459197</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>59</v>
+      </c>
+      <c r="B123" t="s">
+        <v>60</v>
+      </c>
+      <c r="C123" t="s">
+        <v>9</v>
+      </c>
+      <c r="D123">
+        <v>0.70490786676116202</v>
+      </c>
+      <c r="E123">
+        <v>0.67521367521367504</v>
+      </c>
+      <c r="F123">
+        <v>0.530864197530864</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>59</v>
+      </c>
+      <c r="B124" t="s">
+        <v>60</v>
+      </c>
+      <c r="C124" t="s">
+        <v>10</v>
+      </c>
+      <c r="D124">
+        <v>0.61435248002412102</v>
+      </c>
+      <c r="E124">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="F124">
+        <v>0.24793388429752</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>59</v>
+      </c>
+      <c r="B125" t="s">
+        <v>60</v>
+      </c>
+      <c r="C125" t="s">
+        <v>11</v>
+      </c>
+      <c r="D125">
+        <v>0.63562610229276895</v>
+      </c>
+      <c r="E125">
+        <v>0.55982905982905895</v>
+      </c>
+      <c r="F125">
+        <v>0.36024844720496801</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>59</v>
+      </c>
+      <c r="B126" t="s">
+        <v>60</v>
+      </c>
+      <c r="C126" t="s">
+        <v>12</v>
+      </c>
+      <c r="D126">
+        <v>0.65475020109035598</v>
+      </c>
+      <c r="E126">
+        <v>0.62393162393162305</v>
+      </c>
+      <c r="F126">
+        <v>0.52688172043010695</v>
       </c>
     </row>
   </sheetData>

</xml_diff>